<commit_message>
Improvements to db and play mechanics
</commit_message>
<xml_diff>
--- a/DB/ARI_Bell_Heath.xlsx
+++ b/DB/ARI_Bell_Heath.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>lastname</t>
   </si>
@@ -41,6 +41,66 @@
     <t>play_vsrh</t>
   </si>
   <si>
+    <t>bfsp</t>
+  </si>
+  <si>
+    <t>bfrp</t>
+  </si>
+  <si>
+    <t>rest0</t>
+  </si>
+  <si>
+    <t>rest1</t>
+  </si>
+  <si>
+    <t>rest2</t>
+  </si>
+  <si>
+    <t>rest3</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>rnge</t>
+  </si>
+  <si>
+    <t>hold</t>
+  </si>
+  <si>
+    <t>wp</t>
+  </si>
+  <si>
+    <t>balk</t>
+  </si>
+  <si>
+    <t>pickoff</t>
+  </si>
+  <si>
+    <t>durability</t>
+  </si>
+  <si>
+    <t>dldays</t>
+  </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>bunt</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>steal</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>wild</t>
+  </si>
+  <si>
     <t>bell</t>
   </si>
   <si>
@@ -54,6 +114,27 @@
   </si>
   <si>
     <t>park</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Vg_0</t>
+  </si>
+  <si>
+    <t>unlikely</t>
+  </si>
+  <si>
+    <t>rare</t>
+  </si>
+  <si>
+    <t>rsp#1_pr</t>
+  </si>
+  <si>
+    <t>Fr_-1</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
   <si>
     <t>wp_pb</t>
@@ -207,10 +288,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -243,19 +324,79 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>514</v>
@@ -264,10 +405,70 @@
         <v>514</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,10 +479,10 @@
         <v>539</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,10 +493,10 @@
         <v>558</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,10 +507,10 @@
         <v>607</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,10 +521,10 @@
         <v>616</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,10 +535,10 @@
         <v>621</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,10 +549,10 @@
         <v>625</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,10 +563,10 @@
         <v>655</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,10 +577,10 @@
         <v>657</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -390,10 +591,10 @@
         <v>662</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,10 +605,10 @@
         <v>664</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,10 +619,10 @@
         <v>670</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,10 +633,10 @@
         <v>700</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,10 +647,10 @@
         <v>710</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,10 +661,10 @@
         <v>815</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,10 +675,10 @@
         <v>974</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,10 +689,10 @@
         <v>985</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,10 +703,10 @@
         <v>999</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made some more headway on play mechanics.
</commit_message>
<xml_diff>
--- a/DB/ARI_Bell_Heath.xlsx
+++ b/DB/ARI_Bell_Heath.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>lastname</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>steal</t>
-  </si>
-  <si>
-    <t>ab</t>
   </si>
   <si>
     <t>wild</t>
@@ -288,10 +285,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+      <selection pane="topLeft" activeCell="AA1" activeCellId="0" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -381,22 +378,19 @@
       <c r="AA1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>514</v>
@@ -405,10 +399,10 @@
         <v>514</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>0</v>
@@ -432,16 +426,16 @@
         <v>4</v>
       </c>
       <c r="P2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="T2" s="0" t="n">
         <v>0</v>
@@ -453,10 +447,10 @@
         <v>0</v>
       </c>
       <c r="W2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="Y2" s="0" t="n">
         <v>0</v>
@@ -464,11 +458,8 @@
       <c r="Z2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AA2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>39</v>
+      <c r="AA2" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,10 +470,10 @@
         <v>539</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,10 +484,10 @@
         <v>558</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,10 +498,10 @@
         <v>607</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,10 +512,10 @@
         <v>616</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,10 +526,10 @@
         <v>621</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,10 +540,10 @@
         <v>625</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,10 +554,10 @@
         <v>655</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,10 +568,10 @@
         <v>657</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,10 +582,10 @@
         <v>662</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,10 +596,10 @@
         <v>664</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,10 +610,10 @@
         <v>670</v>
       </c>
       <c r="G13" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,10 +624,10 @@
         <v>700</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,10 +638,10 @@
         <v>710</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,10 +652,10 @@
         <v>815</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,10 +666,10 @@
         <v>974</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,10 +680,10 @@
         <v>985</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,10 +694,10 @@
         <v>999</v>
       </c>
       <c r="G19" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>